<commit_message>
-interaction matrix complete, missing bayes testing
</commit_message>
<xml_diff>
--- a/data_files/etc_ch4_rxns.xlsx
+++ b/data_files/etc_ch4_rxns.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="140">
   <si>
     <t xml:space="preserve">Complex I </t>
   </si>
@@ -30,7 +30,7 @@
     <t xml:space="preserve">|NADH-DEHYDROG-A-RXN| </t>
   </si>
   <si>
-    <t xml:space="preserve">|NADH|_cy + 7 |PROTON|_cy + |Ubiquinones|_it --&gt; |NAD|_cy + 6 |PROTON|_pe + |Ubiquinols|_it</t>
+    <t xml:space="preserve">|NADH|_cy + 5 |PROTON|_cy + |Ubiquinones|_it --&gt; |NAD|_cy + 4 |PROTON|_pe + |Ubiquinols|_it</t>
   </si>
   <si>
     <t xml:space="preserve">Complex II</t>
@@ -201,7 +201,7 @@
     <t xml:space="preserve">Carbon Monoxide Dehydrogenase</t>
   </si>
   <si>
-    <t xml:space="preserve">|RXN-11236|</t>
+    <t xml:space="preserve">|RXN-11236| RXN-15838</t>
   </si>
   <si>
     <t xml:space="preserve">Denitrification</t>
@@ -226,6 +226,222 @@
   </si>
   <si>
     <t xml:space="preserve">Methylaspartate Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|ATP-CITRATE-PRO-S--LYASE-RXN|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reductive TCA (CO2 fixation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">|2-OXOGLUTARATE-SYNTHASE-RXN|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R601-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXN-2961</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gluthathion Dependant Formaldehyde Oxidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIBULOSE-BISPHOSPHATE-CARBOXYLASE-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXN-11489</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrate dependent Methane Oxidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PYRUFLAVREDUCT-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lb = -100, ub = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanced cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXN_2961</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lb = 0, ub = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIR, Meis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROPIONMET-PWY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added Full pathway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propionil-coa to succ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROPIONATE__COA_LIGASE_RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanced Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUTYRYL_COA_DEHYDROGENASE_RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLY3KIN-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pathway not realistic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">METHYLENETHFDEHYDROG_NADP_RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formate Balanced Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1.3.1-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxaloacetate Balanced Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXN-2802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spurious Glyoxylate Regeneration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R10-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RumP Formaldehyde Assimilation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISOCIT-CLEAV-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glyoxylate Shunt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nitrate Dependent Methane Oxidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CITSYN-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lb = 0, ub = 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCA direcionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXN-20917</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyruvate Balance cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EX_METOH_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methanol Production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLUTAMATE-DEHYDROGENASE-NADP+-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glutamate Balanced Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXN-12168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Succ Balanced cycle in Methylaspartate Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R125-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acetyl-Coa Balanced cyacle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLUTACONYL-COA-DECARBOXYLASE-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crotonyl-Coa Balanced cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUTTRANSAM-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXN-15125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXNI-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malate Balanced Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXN-7774</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXNI-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCVMULTI-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glutamate Ammonium Balanced Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXN-7566</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ammonium Balanced cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASPARTASE-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLUTAMATE-DEHYDROGENASE-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KETOGLUTREDUCT-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxoglutarate Balanced cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXN-11662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acetoaceyl-CoA Balanced Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-METHYLCITRATE-SYNTHASE-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RXN0-268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propionil-coa Balanced Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEPSYNTH-RXN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyruvate balanced Cycle</t>
   </si>
 </sst>
 </file>
@@ -235,7 +451,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -263,6 +479,18 @@
       <name val="Ubuntu"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -307,7 +535,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -321,6 +549,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -403,8 +643,8 @@
   </sheetPr>
   <dimension ref="A3:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -829,16 +1069,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.93"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -888,6 +1129,7 @@
       <c r="B6" s="0" t="s">
         <v>60</v>
       </c>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -921,7 +1163,536 @@
         <v>67</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B11:B13"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>